<commit_message>
CS-262 Homework 3 Materials Added.
</commit_message>
<xml_diff>
--- a/Team Member Review.xlsx
+++ b/Team Member Review.xlsx
@@ -9,18 +9,19 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25560" windowHeight="17025" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25560" windowHeight="17025" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="57">
   <si>
     <t>Communication</t>
   </si>
@@ -146,6 +147,51 @@
   </si>
   <si>
     <t>Passion is constrained by our time constraints as we all have 3-4 other classes to worry about.</t>
+  </si>
+  <si>
+    <t>Good luck on your soccer game this Friday while we do our presentations ;D</t>
+  </si>
+  <si>
+    <t>Thanks for constructing our relational database schema upon which I built our RESTful web service and CRUD test activities</t>
+  </si>
+  <si>
+    <t>Thanks for constructing our PowerPoint Slide for the presentation on Friday.  Everybody gave it a thumbs up of approval seal.</t>
+  </si>
+  <si>
+    <t>Having someone in CIT who knows how to operator the projector and computer systems around campus is definitely useful when making sure we encounter no technical hiccups with the equipment for the presentation.</t>
+  </si>
+  <si>
+    <t>Thanks for adding back-end integration with our Sport Table to the Sport Selection Activity.  Good luck on integrating Google Oauth with our back-end.</t>
+  </si>
+  <si>
+    <t>I'd say we're pretty good at communicating via Slack now.  People seem to know to use @INSERTNAMEHERE to get someone's attention.</t>
+  </si>
+  <si>
+    <t>We're still never totally on topic during conversations, there's always tangential topics now and again.</t>
+  </si>
+  <si>
+    <t>I'd say we're functioning conflict-free throughout the semester.  No clashing personalities that I've noticed.</t>
+  </si>
+  <si>
+    <t>We have Bolu, Caleb, and Ian C. on updating and maintaining the non-coding related activites for our project while me, Mark, and Ian A. update and maintain the coding related activities for our project.</t>
+  </si>
+  <si>
+    <t>There's some overlap as we've all contributed in some part to all aspects of the project, but for the most part that's how we've divded the work.</t>
+  </si>
+  <si>
+    <t>Numerically, it's not equal, but sometimes you get stuck on a bug that you can't fix for hours on end &gt;_&gt;.  So, in the end, it evens out in terms of actual work done.  I might have binged a little too much the past week, voluntarily.</t>
+  </si>
+  <si>
+    <t>We're all willing to answer questions when someone asks, as long as its within our breadth of knowledge.</t>
+  </si>
+  <si>
+    <t>Scheduling conflicts are unavoidable.  People's class schedule and other obligations sometimes prevent part of the team from showing up exactly on time.  But, we manage to communicate what's going on to everyone in the end.</t>
+  </si>
+  <si>
+    <t>I'd say we're meeting deadlines pretty well so far based on instructor critiques and evaluations.</t>
+  </si>
+  <si>
+    <t>Passion is always mitigated by having to worry about 3-4 other classes and micro-managing time investment in each of our classes.</t>
   </si>
 </sst>
 </file>
@@ -205,7 +251,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -225,6 +271,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -544,7 +594,7 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="15" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -568,7 +618,7 @@
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A3" s="14"/>
+      <c r="A3" s="16"/>
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
@@ -590,7 +640,7 @@
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="14"/>
+      <c r="A4" s="16"/>
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
@@ -612,7 +662,7 @@
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="15" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -636,7 +686,7 @@
       <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="14"/>
+      <c r="A6" s="16"/>
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
@@ -660,7 +710,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A7" s="14"/>
+      <c r="A7" s="16"/>
       <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
@@ -682,7 +732,7 @@
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="15" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -706,7 +756,7 @@
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="14"/>
+      <c r="A9" s="16"/>
       <c r="B9" s="1" t="s">
         <v>10</v>
       </c>
@@ -728,7 +778,7 @@
       <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="14"/>
+      <c r="A10" s="16"/>
       <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
@@ -809,8 +859,8 @@
   </sheetPr>
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D24" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -847,7 +897,7 @@
       <c r="K1" s="11"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="15" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -874,7 +924,7 @@
       <c r="K2" s="11"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="14"/>
+      <c r="A3" s="16"/>
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
@@ -899,7 +949,7 @@
       <c r="K3" s="11"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="14"/>
+      <c r="A4" s="16"/>
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
@@ -924,7 +974,7 @@
       <c r="K4" s="11"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="15" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -951,7 +1001,7 @@
       <c r="K5" s="11"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="14"/>
+      <c r="A6" s="16"/>
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
@@ -978,7 +1028,7 @@
       <c r="K6" s="11"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="14"/>
+      <c r="A7" s="16"/>
       <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
@@ -1003,7 +1053,7 @@
       <c r="K7" s="11"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="15" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -1030,7 +1080,7 @@
       <c r="K8" s="11"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="14"/>
+      <c r="A9" s="16"/>
       <c r="B9" s="1" t="s">
         <v>10</v>
       </c>
@@ -1055,7 +1105,7 @@
       <c r="K9" s="11"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="14"/>
+      <c r="A10" s="16"/>
       <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
@@ -1221,4 +1271,333 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="53" orientation="landscape" horizontalDpi="4294967293" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:H22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.140625" style="14" customWidth="1"/>
+    <col min="2" max="2" width="46.5703125" style="14" customWidth="1"/>
+    <col min="3" max="4" width="27" style="14" customWidth="1"/>
+    <col min="5" max="5" width="31.85546875" style="14" customWidth="1"/>
+    <col min="6" max="6" width="26.28515625" style="14" customWidth="1"/>
+    <col min="7" max="7" width="28.140625" style="14" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="14"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1">
+        <v>5</v>
+      </c>
+      <c r="E2" s="1">
+        <v>5</v>
+      </c>
+      <c r="F2" s="1">
+        <v>5</v>
+      </c>
+      <c r="G2" s="1">
+        <v>5</v>
+      </c>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="16"/>
+      <c r="B3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1">
+        <v>4</v>
+      </c>
+      <c r="D3" s="1">
+        <v>4</v>
+      </c>
+      <c r="E3" s="1">
+        <v>4</v>
+      </c>
+      <c r="F3" s="1">
+        <v>4</v>
+      </c>
+      <c r="G3" s="1">
+        <v>4</v>
+      </c>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="16"/>
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1">
+        <v>5</v>
+      </c>
+      <c r="D4" s="1">
+        <v>5</v>
+      </c>
+      <c r="E4" s="1">
+        <v>5</v>
+      </c>
+      <c r="F4" s="1">
+        <v>5</v>
+      </c>
+      <c r="G4" s="1">
+        <v>5</v>
+      </c>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1">
+        <v>5</v>
+      </c>
+      <c r="D5" s="1">
+        <v>5</v>
+      </c>
+      <c r="E5" s="1">
+        <v>5</v>
+      </c>
+      <c r="F5" s="1">
+        <v>5</v>
+      </c>
+      <c r="G5" s="1">
+        <v>5</v>
+      </c>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="16"/>
+      <c r="B6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0.16666666669999999</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0.16666666669999999</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0.16666666669999999</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0.16666666669999999</v>
+      </c>
+      <c r="G6" s="7">
+        <v>0.16666666669999999</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="16"/>
+      <c r="B7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="1">
+        <v>5</v>
+      </c>
+      <c r="D7" s="1">
+        <v>5</v>
+      </c>
+      <c r="E7" s="1">
+        <v>5</v>
+      </c>
+      <c r="F7" s="1">
+        <v>5</v>
+      </c>
+      <c r="G7" s="1">
+        <v>5</v>
+      </c>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="1">
+        <v>4</v>
+      </c>
+      <c r="D8" s="1">
+        <v>4</v>
+      </c>
+      <c r="E8" s="1">
+        <v>4</v>
+      </c>
+      <c r="F8" s="1">
+        <v>4</v>
+      </c>
+      <c r="G8" s="1">
+        <v>4</v>
+      </c>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="16"/>
+      <c r="B9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="1">
+        <v>5</v>
+      </c>
+      <c r="D9" s="1">
+        <v>5</v>
+      </c>
+      <c r="E9" s="1">
+        <v>5</v>
+      </c>
+      <c r="F9" s="1">
+        <v>5</v>
+      </c>
+      <c r="G9" s="1">
+        <v>5</v>
+      </c>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="16"/>
+      <c r="B10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="1">
+        <v>4</v>
+      </c>
+      <c r="D10" s="1">
+        <v>4</v>
+      </c>
+      <c r="E10" s="1">
+        <v>4</v>
+      </c>
+      <c r="F10" s="1">
+        <v>4</v>
+      </c>
+      <c r="G10" s="1">
+        <v>4</v>
+      </c>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" ht="114.75" x14ac:dyDescent="0.2">
+      <c r="A11" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="12" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" s="12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" s="12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="A8:A10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="53" fitToHeight="0" orientation="landscape" horizontalDpi="4294967293" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
CS-262: Guide 12 Finished.
</commit_message>
<xml_diff>
--- a/Team Member Review.xlsx
+++ b/Team Member Review.xlsx
@@ -5,23 +5,24 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Calvin College\Fall Semester 2018\CS 262\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\CS_262\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25560" windowHeight="17025" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25560" windowHeight="17025" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="57">
   <si>
     <t>Communication</t>
   </si>
@@ -251,7 +252,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -271,6 +272,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -594,7 +599,7 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="17" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -618,7 +623,7 @@
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A3" s="16"/>
+      <c r="A3" s="18"/>
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
@@ -640,7 +645,7 @@
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="16"/>
+      <c r="A4" s="18"/>
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
@@ -662,7 +667,7 @@
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="17" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -686,7 +691,7 @@
       <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="16"/>
+      <c r="A6" s="18"/>
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
@@ -710,7 +715,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A7" s="16"/>
+      <c r="A7" s="18"/>
       <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
@@ -732,7 +737,7 @@
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="17" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -756,7 +761,7 @@
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="16"/>
+      <c r="A9" s="18"/>
       <c r="B9" s="1" t="s">
         <v>10</v>
       </c>
@@ -778,7 +783,7 @@
       <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="16"/>
+      <c r="A10" s="18"/>
       <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
@@ -897,7 +902,7 @@
       <c r="K1" s="11"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="17" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -924,7 +929,7 @@
       <c r="K2" s="11"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="16"/>
+      <c r="A3" s="18"/>
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
@@ -949,7 +954,7 @@
       <c r="K3" s="11"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="16"/>
+      <c r="A4" s="18"/>
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
@@ -974,7 +979,7 @@
       <c r="K4" s="11"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="17" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1001,7 +1006,7 @@
       <c r="K5" s="11"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="16"/>
+      <c r="A6" s="18"/>
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
@@ -1028,7 +1033,7 @@
       <c r="K6" s="11"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="16"/>
+      <c r="A7" s="18"/>
       <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
@@ -1053,7 +1058,7 @@
       <c r="K7" s="11"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="17" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -1080,7 +1085,7 @@
       <c r="K8" s="11"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="16"/>
+      <c r="A9" s="18"/>
       <c r="B9" s="1" t="s">
         <v>10</v>
       </c>
@@ -1105,7 +1110,7 @@
       <c r="K9" s="11"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="16"/>
+      <c r="A10" s="18"/>
       <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
@@ -1280,7 +1285,9 @@
   </sheetPr>
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1314,7 +1321,7 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="17" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1338,7 +1345,7 @@
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="16"/>
+      <c r="A3" s="18"/>
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1360,7 +1367,7 @@
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="16"/>
+      <c r="A4" s="18"/>
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1382,7 +1389,7 @@
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="17" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1406,7 +1413,7 @@
       <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="16"/>
+      <c r="A6" s="18"/>
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
@@ -1430,7 +1437,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="16"/>
+      <c r="A7" s="18"/>
       <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
@@ -1452,7 +1459,7 @@
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="17" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -1476,7 +1483,7 @@
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="16"/>
+      <c r="A9" s="18"/>
       <c r="B9" s="1" t="s">
         <v>10</v>
       </c>
@@ -1498,7 +1505,7 @@
       <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="16"/>
+      <c r="A10" s="18"/>
       <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
@@ -1524,8 +1531,8 @@
         <v>12</v>
       </c>
       <c r="B11" s="1"/>
-      <c r="C11" s="9" t="s">
-        <v>42</v>
+      <c r="C11" s="1">
+        <v>4</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>43</v>
@@ -1600,4 +1607,331 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="53" fitToHeight="0" orientation="landscape" horizontalDpi="4294967293" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.140625" style="16" customWidth="1"/>
+    <col min="2" max="2" width="46.5703125" style="16" customWidth="1"/>
+    <col min="3" max="4" width="27" style="16" customWidth="1"/>
+    <col min="5" max="5" width="31.85546875" style="16" customWidth="1"/>
+    <col min="6" max="6" width="26.28515625" style="16" customWidth="1"/>
+    <col min="7" max="7" width="28.140625" style="16" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="16"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1">
+        <v>5</v>
+      </c>
+      <c r="E2" s="1">
+        <v>5</v>
+      </c>
+      <c r="F2" s="1">
+        <v>5</v>
+      </c>
+      <c r="G2" s="1">
+        <v>5</v>
+      </c>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="18"/>
+      <c r="B3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1">
+        <v>4</v>
+      </c>
+      <c r="D3" s="1">
+        <v>4</v>
+      </c>
+      <c r="E3" s="1">
+        <v>4</v>
+      </c>
+      <c r="F3" s="1">
+        <v>4</v>
+      </c>
+      <c r="G3" s="1">
+        <v>4</v>
+      </c>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="18"/>
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1">
+        <v>5</v>
+      </c>
+      <c r="D4" s="1">
+        <v>5</v>
+      </c>
+      <c r="E4" s="1">
+        <v>5</v>
+      </c>
+      <c r="F4" s="1">
+        <v>5</v>
+      </c>
+      <c r="G4" s="1">
+        <v>5</v>
+      </c>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1">
+        <v>5</v>
+      </c>
+      <c r="D5" s="1">
+        <v>5</v>
+      </c>
+      <c r="E5" s="1">
+        <v>5</v>
+      </c>
+      <c r="F5" s="1">
+        <v>5</v>
+      </c>
+      <c r="G5" s="1">
+        <v>5</v>
+      </c>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="18"/>
+      <c r="B6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0.16666666669999999</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0.16666666669999999</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0.16666666669999999</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0.16666666669999999</v>
+      </c>
+      <c r="G6" s="7">
+        <v>0.16666666669999999</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="18"/>
+      <c r="B7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="1">
+        <v>5</v>
+      </c>
+      <c r="D7" s="1">
+        <v>5</v>
+      </c>
+      <c r="E7" s="1">
+        <v>5</v>
+      </c>
+      <c r="F7" s="1">
+        <v>5</v>
+      </c>
+      <c r="G7" s="1">
+        <v>5</v>
+      </c>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="1">
+        <v>4</v>
+      </c>
+      <c r="D8" s="1">
+        <v>4</v>
+      </c>
+      <c r="E8" s="1">
+        <v>4</v>
+      </c>
+      <c r="F8" s="1">
+        <v>4</v>
+      </c>
+      <c r="G8" s="1">
+        <v>4</v>
+      </c>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="18"/>
+      <c r="B9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="1">
+        <v>5</v>
+      </c>
+      <c r="D9" s="1">
+        <v>5</v>
+      </c>
+      <c r="E9" s="1">
+        <v>5</v>
+      </c>
+      <c r="F9" s="1">
+        <v>5</v>
+      </c>
+      <c r="G9" s="1">
+        <v>5</v>
+      </c>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="18"/>
+      <c r="B10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="1">
+        <v>4</v>
+      </c>
+      <c r="D10" s="1">
+        <v>4</v>
+      </c>
+      <c r="E10" s="1">
+        <v>4</v>
+      </c>
+      <c r="F10" s="1">
+        <v>4</v>
+      </c>
+      <c r="G10" s="1">
+        <v>4</v>
+      </c>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" ht="114.75" x14ac:dyDescent="0.2">
+      <c r="A11" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="12" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" s="12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" s="12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="A8:A10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
CS-262: Team Member Review and Team Stakeholder Sprint Review finished.
</commit_message>
<xml_diff>
--- a/Team Member Review.xlsx
+++ b/Team Member Review.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="78">
   <si>
     <t>Communication</t>
   </si>
@@ -150,9 +150,6 @@
     <t>Passion is constrained by our time constraints as we all have 3-4 other classes to worry about.</t>
   </si>
   <si>
-    <t>Good luck on your soccer game this Friday while we do our presentations ;D</t>
-  </si>
-  <si>
     <t>Thanks for constructing our relational database schema upon which I built our RESTful web service and CRUD test activities</t>
   </si>
   <si>
@@ -193,6 +190,72 @@
   </si>
   <si>
     <t>Passion is always mitigated by having to worry about 3-4 other classes and micro-managing time investment in each of our classes.</t>
+  </si>
+  <si>
+    <t>Thanks for the hard-work in adding to the RESTful web service API and integrating database requests via Volley in our front-end application.</t>
+  </si>
+  <si>
+    <t>Glad Calvin's soccer team is doing well so far. Thanks for re-factoring segments of code for better style and code hospitality.</t>
+  </si>
+  <si>
+    <t>Thanks for modifying our database schema with more precise names for attributes.</t>
+  </si>
+  <si>
+    <t>Looking forward to seeing your completed revisions to our activity (sport) selection screen, if I'm remembering the correctly.</t>
+  </si>
+  <si>
+    <t>Per usual, thanks for scheduling our team meetings, scheduling availablility for test subjects/stakeholders via Google spreadsheets, and also for writing the initial draft of our usability test script.</t>
+  </si>
+  <si>
+    <t>Scheduling team meetings has become more difficult, and we've had several cancellations due to over half the team not being to make it on a particular day.</t>
+  </si>
+  <si>
+    <t>Slack is the easiest place to communicate with each other for now.</t>
+  </si>
+  <si>
+    <t>We're further ahead on our development of the back-end and front-end than we are with maintaining project documentation.</t>
+  </si>
+  <si>
+    <t>Maintaining quality project documentation just takes that much more additional time away from finishing the basic functionalty of our application.</t>
+  </si>
+  <si>
+    <t>Relating to that, our presentation could have gone better if we had managed to schedule time to practice together rather than just winging it.</t>
+  </si>
+  <si>
+    <t>I am personally more of a creator than an administrator, so I find it far more fun to be creating than maintaining.</t>
+  </si>
+  <si>
+    <t>Passion is hard to maintain as its nearing finals and we're all busy juggling our classes and associated homework/study.</t>
+  </si>
+  <si>
+    <t>We meet deadlines, but the quality of the work, can be a bit rushed due to the time crunch from nearing the end of the semester. (*cough* rough draft of usability test script *cough*)</t>
+  </si>
+  <si>
+    <t>The lab computers are NOT optimal workstations for doing Android Studio development for our team project.</t>
+  </si>
+  <si>
+    <t>We have some personnel system bottlenecks. Only Mark Wissink and I have machines capable of Android development.  Everyone else's system is too outdated and tend to hang up, freeze, or suffer other issues running Android Studio.</t>
+  </si>
+  <si>
+    <t>I am also the only person on the team with a Android Phone available for usability testing and this is my personal phone that has all my 2 factor authentication for bank accounts, etc.</t>
+  </si>
+  <si>
+    <t>This will present issues based on the availability of stakeholders, test subjects, and the team members themselves.</t>
+  </si>
+  <si>
+    <t>Mark and I are the only people with a decent grasp of how to implement and modify our back-end, including the RESTful webservice, integration with front-end Knight-Ranker application, and GCP in general.</t>
+  </si>
+  <si>
+    <t>(well, I did sort of build the code-base foundation for the back-end and front-end)</t>
+  </si>
+  <si>
+    <t>Our issues aside, we're still plodding along and we should at least have a presentable and functional Knight-Ranker application for the final presentation, regardless of how terrible our code-base might look in terms of documentation and styling.</t>
+  </si>
+  <si>
+    <t>The UI model is almost pointless to maintain as we make continual and semi-regular changes to the UI in our application.</t>
+  </si>
+  <si>
+    <t>We need to draft aesthetically pleasing final versions of our domain model, and other more static documents.</t>
   </si>
 </sst>
 </file>
@@ -1535,67 +1598,67 @@
         <v>4</v>
       </c>
       <c r="D11" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="F11" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="F11" s="9" t="s">
+      <c r="G11" s="9" t="s">
         <v>45</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>46</v>
       </c>
       <c r="H11" s="1"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1611,10 +1674,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H22"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1656,16 +1722,16 @@
         <v>1</v>
       </c>
       <c r="C2" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D2" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E2" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F2" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G2" s="1">
         <v>5</v>
@@ -1816,19 +1882,19 @@
         <v>10</v>
       </c>
       <c r="C9" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D9" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E9" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F9" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G9" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H9" s="1"/>
     </row>
@@ -1838,92 +1904,127 @@
         <v>11</v>
       </c>
       <c r="C10" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D10" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E10" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F10" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G10" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="1:8" ht="114.75" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="102" x14ac:dyDescent="0.2">
       <c r="A11" s="15" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="9" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="H11" s="1"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="12" t="s">
-        <v>47</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="12" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="12" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
-        <v>50</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" s="12" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" s="12" t="s">
-        <v>56</v>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" s="12" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" s="12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" s="12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" s="12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" s="12" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" s="12" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" s="12" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1933,5 +2034,6 @@
     <mergeCell ref="A8:A10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="53" fitToHeight="0" orientation="landscape" horizontalDpi="4294967293" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Final templates for semester review added; also screen captures for online help system.
</commit_message>
<xml_diff>
--- a/Team Member Review.xlsx
+++ b/Team Member Review.xlsx
@@ -9,20 +9,21 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25560" windowHeight="17025" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25560" windowHeight="17025" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="79">
   <si>
     <t>Communication</t>
   </si>
@@ -256,6 +257,9 @@
   </si>
   <si>
     <t>We need to draft aesthetically pleasing final versions of our domain model, and other more static documents.</t>
+  </si>
+  <si>
+    <t>I will keep the same values as the previous sprint.  As we keep on nearing finals, everybody's priorities shift towards studying for finals rather than last-minute programming, administration, design, etc., binges for the team project; myself included.</t>
   </si>
 </sst>
 </file>
@@ -315,7 +319,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -335,6 +339,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -662,7 +670,7 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="19" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -686,7 +694,7 @@
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A3" s="18"/>
+      <c r="A3" s="20"/>
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
@@ -708,7 +716,7 @@
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="18"/>
+      <c r="A4" s="20"/>
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
@@ -730,7 +738,7 @@
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="19" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -754,7 +762,7 @@
       <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="18"/>
+      <c r="A6" s="20"/>
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
@@ -778,7 +786,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A7" s="18"/>
+      <c r="A7" s="20"/>
       <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
@@ -800,7 +808,7 @@
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="19" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -824,7 +832,7 @@
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="18"/>
+      <c r="A9" s="20"/>
       <c r="B9" s="1" t="s">
         <v>10</v>
       </c>
@@ -846,7 +854,7 @@
       <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="18"/>
+      <c r="A10" s="20"/>
       <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
@@ -965,7 +973,7 @@
       <c r="K1" s="11"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="19" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -992,7 +1000,7 @@
       <c r="K2" s="11"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="18"/>
+      <c r="A3" s="20"/>
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1017,7 +1025,7 @@
       <c r="K3" s="11"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="18"/>
+      <c r="A4" s="20"/>
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1042,7 +1050,7 @@
       <c r="K4" s="11"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="19" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1069,7 +1077,7 @@
       <c r="K5" s="11"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="18"/>
+      <c r="A6" s="20"/>
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
@@ -1096,7 +1104,7 @@
       <c r="K6" s="11"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="18"/>
+      <c r="A7" s="20"/>
       <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
@@ -1121,7 +1129,7 @@
       <c r="K7" s="11"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="19" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -1148,7 +1156,7 @@
       <c r="K8" s="11"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="18"/>
+      <c r="A9" s="20"/>
       <c r="B9" s="1" t="s">
         <v>10</v>
       </c>
@@ -1173,7 +1181,7 @@
       <c r="K9" s="11"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="18"/>
+      <c r="A10" s="20"/>
       <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
@@ -1384,7 +1392,7 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="19" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1408,7 +1416,7 @@
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="18"/>
+      <c r="A3" s="20"/>
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1430,7 +1438,7 @@
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="18"/>
+      <c r="A4" s="20"/>
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1452,7 +1460,7 @@
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="19" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1476,7 +1484,7 @@
       <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="18"/>
+      <c r="A6" s="20"/>
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
@@ -1500,7 +1508,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="18"/>
+      <c r="A7" s="20"/>
       <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
@@ -1522,7 +1530,7 @@
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="19" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -1546,7 +1554,7 @@
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="18"/>
+      <c r="A9" s="20"/>
       <c r="B9" s="1" t="s">
         <v>10</v>
       </c>
@@ -1568,7 +1576,7 @@
       <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="18"/>
+      <c r="A10" s="20"/>
       <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
@@ -1679,8 +1687,8 @@
   </sheetPr>
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C37" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1715,7 +1723,7 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="19" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1739,7 +1747,7 @@
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="18"/>
+      <c r="A3" s="20"/>
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1761,7 +1769,7 @@
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="18"/>
+      <c r="A4" s="20"/>
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1783,7 +1791,7 @@
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="19" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1807,7 +1815,7 @@
       <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="18"/>
+      <c r="A6" s="20"/>
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
@@ -1831,7 +1839,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="18"/>
+      <c r="A7" s="20"/>
       <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
@@ -1853,7 +1861,7 @@
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="19" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -1877,7 +1885,7 @@
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="18"/>
+      <c r="A9" s="20"/>
       <c r="B9" s="1" t="s">
         <v>10</v>
       </c>
@@ -1899,7 +1907,7 @@
       <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="18"/>
+      <c r="A10" s="20"/>
       <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
@@ -2036,4 +2044,324 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="53" fitToHeight="0" orientation="landscape" horizontalDpi="4294967293" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.140625" style="18" customWidth="1"/>
+    <col min="2" max="2" width="46.5703125" style="18" customWidth="1"/>
+    <col min="3" max="4" width="27" style="18" customWidth="1"/>
+    <col min="5" max="5" width="31.85546875" style="18" customWidth="1"/>
+    <col min="6" max="6" width="26.28515625" style="18" customWidth="1"/>
+    <col min="7" max="7" width="28.140625" style="18" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="18"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1">
+        <v>4</v>
+      </c>
+      <c r="E2" s="1">
+        <v>4</v>
+      </c>
+      <c r="F2" s="1">
+        <v>4</v>
+      </c>
+      <c r="G2" s="1">
+        <v>5</v>
+      </c>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="20"/>
+      <c r="B3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1">
+        <v>4</v>
+      </c>
+      <c r="D3" s="1">
+        <v>4</v>
+      </c>
+      <c r="E3" s="1">
+        <v>4</v>
+      </c>
+      <c r="F3" s="1">
+        <v>4</v>
+      </c>
+      <c r="G3" s="1">
+        <v>4</v>
+      </c>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="20"/>
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1">
+        <v>5</v>
+      </c>
+      <c r="D4" s="1">
+        <v>5</v>
+      </c>
+      <c r="E4" s="1">
+        <v>5</v>
+      </c>
+      <c r="F4" s="1">
+        <v>5</v>
+      </c>
+      <c r="G4" s="1">
+        <v>5</v>
+      </c>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1">
+        <v>5</v>
+      </c>
+      <c r="D5" s="1">
+        <v>5</v>
+      </c>
+      <c r="E5" s="1">
+        <v>5</v>
+      </c>
+      <c r="F5" s="1">
+        <v>5</v>
+      </c>
+      <c r="G5" s="1">
+        <v>5</v>
+      </c>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="20"/>
+      <c r="B6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0.16666666669999999</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0.16666666669999999</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0.16666666669999999</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0.16666666669999999</v>
+      </c>
+      <c r="G6" s="7">
+        <v>0.16666666669999999</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="20"/>
+      <c r="B7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="1">
+        <v>5</v>
+      </c>
+      <c r="D7" s="1">
+        <v>5</v>
+      </c>
+      <c r="E7" s="1">
+        <v>5</v>
+      </c>
+      <c r="F7" s="1">
+        <v>5</v>
+      </c>
+      <c r="G7" s="1">
+        <v>5</v>
+      </c>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="1">
+        <v>4</v>
+      </c>
+      <c r="D8" s="1">
+        <v>4</v>
+      </c>
+      <c r="E8" s="1">
+        <v>4</v>
+      </c>
+      <c r="F8" s="1">
+        <v>4</v>
+      </c>
+      <c r="G8" s="1">
+        <v>4</v>
+      </c>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="20"/>
+      <c r="B9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="1">
+        <v>4</v>
+      </c>
+      <c r="D9" s="1">
+        <v>4</v>
+      </c>
+      <c r="E9" s="1">
+        <v>4</v>
+      </c>
+      <c r="F9" s="1">
+        <v>4</v>
+      </c>
+      <c r="G9" s="1">
+        <v>4</v>
+      </c>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="20"/>
+      <c r="B10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="1">
+        <v>3</v>
+      </c>
+      <c r="D10" s="1">
+        <v>3</v>
+      </c>
+      <c r="E10" s="1">
+        <v>3</v>
+      </c>
+      <c r="F10" s="1">
+        <v>3</v>
+      </c>
+      <c r="G10" s="1">
+        <v>3</v>
+      </c>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="12" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="12"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="12"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="12"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="12"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="12"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="12"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" s="12"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" s="12"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" s="12"/>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" s="12"/>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" s="12"/>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" s="12"/>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" s="12"/>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" s="12"/>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" s="12"/>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" s="12"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="A8:A10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Began Sprint 5 Final Reviews for CS-262.
</commit_message>
<xml_diff>
--- a/Team Member Review.xlsx
+++ b/Team Member Review.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25560" windowHeight="17025" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24840" windowHeight="1395" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="115">
   <si>
     <t>Communication</t>
   </si>
@@ -260,6 +260,114 @@
   </si>
   <si>
     <t>I will keep the same values as the previous sprint.  As we keep on nearing finals, everybody's priorities shift towards studying for finals rather than last-minute programming, administration, design, etc., binges for the team project; myself included.</t>
+  </si>
+  <si>
+    <t>In CS-212, we saw you flash by the camera when we watched your soccer match for the first few minutes of class ;D</t>
+  </si>
+  <si>
+    <t>Thanks for updating the UI model and creating the Deployment Diagram.</t>
+  </si>
+  <si>
+    <t>Thanks for creating the PowerPoint presentation slides for our final presentation and also your work on the Resolve Matches screen.</t>
+  </si>
+  <si>
+    <t>Thanks for all the work you did for our Usability Testing, Script, and Report, as well as other miscellaneous administrative tasks.</t>
+  </si>
+  <si>
+    <t>Thanks for updating and modifying the RESTful web service and integrating core features of the application to work with our back-end.</t>
+  </si>
+  <si>
+    <t>Our passions has to be evenly distrubted across all our classes this semester so as to maintain a satisfactory G.P.A.</t>
+  </si>
+  <si>
+    <t>We deprecated full team meetings the past few weeks due to scheduling conflicts.</t>
+  </si>
+  <si>
+    <t>We have run out of funding twice now on GCP, the third coupon code should last till past final presentations.</t>
+  </si>
+  <si>
+    <t>I think I am the only person with a powerful enough laptop to run Android Studio without resource issues - lag, long load times, crashes, etc.</t>
+  </si>
+  <si>
+    <t>I wish I had more free time towards the end of the semester to go on programming binges but my part-time job at the Thai Restaurant started back up after the renovation was finished after that little fire incident that occurred in January.</t>
+  </si>
+  <si>
+    <t>This 2nd experience of working on a team for software development (my first being the Thailand interim) has definitely improved my working knowledge of GitFlow, Git, GitHub, etc.</t>
+  </si>
+  <si>
+    <t>Understandably, Bolu and Caleb would prefer to work on non-coding tasks as their interest lean towards data science and information technology, respectively.</t>
+  </si>
+  <si>
+    <t>I definitely enjoyed "greenfield" development by creating the code-base foundation for the Android App and RESTful web service as well as Gloogle Cloud Platform deployment.</t>
+  </si>
+  <si>
+    <t>It provided me with a nice working knowledge of all aspects of the project, which allowed me to multi-task and jump from one task to another, without being completely lost.</t>
+  </si>
+  <si>
+    <t>Mark definitely did quite a bit of work to update the RESTful web service and database schema and implement the Volley network library to provide a easier way of communicating with the web service.</t>
+  </si>
+  <si>
+    <t>Caleb generated the initial draft of our database schema upon which we based future revisions upon.</t>
+  </si>
+  <si>
+    <t>Ian C. made his best attempt to jump into our code-base despite not having been involved in the initial foundation.  It's definitely difficult to analyze and understand existing code, even if it is decently documented.</t>
+  </si>
+  <si>
+    <t>Ian A. had soccer obligations so he had to shift his priorities elsewhere for a while.</t>
+  </si>
+  <si>
+    <t>I think we got along just fine as a team overall.  I didn't really see any personality conflicts.  We all have a sense of humor.</t>
+  </si>
+  <si>
+    <t>There's always that last minute push to implement additional features, bugfixes, or update documentations, before the end of every sprint when deliverables are due.</t>
+  </si>
+  <si>
+    <t>Work hours doesn't necessarily equate to work completed, as oft-times those hours involve extensive research on how to resolve an issue or implement a feature.</t>
+  </si>
+  <si>
+    <t>The actual writing of code usually doesn't take anywhere near as long as figuring out how to implement the functionality.</t>
+  </si>
+  <si>
+    <t>It's definitely correct to say that after a couple weeks your own code starts to look as alien as someone else's code.  It took me a while to re-acclimate to my own code after a extended time of leave from that particular segment.</t>
+  </si>
+  <si>
+    <t>Android Studio is definitely a powerful IDE, I just wish Google had better up-to-date documentation on it.</t>
+  </si>
+  <si>
+    <t>Some of our team members might have significantly less recorded hours than Mark or I, but they still completed tasks that were essential to getting a good grade and producing the necessary deliverables.</t>
+  </si>
+  <si>
+    <t>I'm pretty sure people forgot to record all their hours spent on the project.  I did a pretty good job of recording every minute on spent.</t>
+  </si>
+  <si>
+    <t>It actually takes a while to write a proper commit message that documents your changes, update Trello to reflect the tasks in-progress/backlogged/finished, etc., and even longer if you're documenting your code on-the-fly as you code.</t>
+  </si>
+  <si>
+    <t>I tried using the GitHub issue tracker to document bugs, coding-related tasks, etc., and to use "Resolves #61" in my pull requests.</t>
+  </si>
+  <si>
+    <t>My coffee intake has steadily increased as finals near, per the norm.  It's to the point where I feel lethargic in the morning without gulping dodwn a cup first thing.  Looking forward to the coffee migraines at the end.</t>
+  </si>
+  <si>
+    <t>I fee like software egnineering should be a two semester classes, ideally.  There simply isn't enough time in one semester with everyone having 4-5 classes to worry about to commit enough time to create a decent product.</t>
+  </si>
+  <si>
+    <t>I definitely think I'm in the right major/program since I can definitely sit in front of a monitor and code for 10 hours straight, provided I have enough coffee to sustain me.</t>
+  </si>
+  <si>
+    <t>It's still somewhat fun to update Trello and GitHub and other project management tools.</t>
+  </si>
+  <si>
+    <t>It's hard to be purely cold and objective when you've gotten to know your team members well and like them.</t>
+  </si>
+  <si>
+    <t>Caleb and Boly were purely on the non-coding related tasks.  Ian C. was sort of a hybrid of the two.  Ian A. leaned more towards the coding.  Mark and I were heavily on the coding tasks.</t>
+  </si>
+  <si>
+    <t>I provided the Android smartphone for usability testing and general demo purposes as everyone else apparently owns an Iphone on the team.</t>
+  </si>
+  <si>
+    <t>Overall, when push comes to shove, we get things done, one way or another, for better or worse.</t>
   </si>
 </sst>
 </file>
@@ -2048,10 +2156,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H29"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:H44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2291,16 +2402,26 @@
       </c>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A11" s="17" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="1"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
+      <c r="C11" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>83</v>
+      </c>
       <c r="H11" s="1"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -2309,52 +2430,159 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="12"/>
+      <c r="A14" s="12" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="12"/>
+      <c r="A15" s="12" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="12"/>
+      <c r="A16" s="12" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="12"/>
+      <c r="A17" s="12" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="12"/>
+      <c r="A18" s="12" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="12"/>
+      <c r="A19" s="12" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="12"/>
+      <c r="A20" s="12" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" s="12"/>
+      <c r="A21" s="12" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" s="12"/>
+      <c r="A22" s="12" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" s="12"/>
+      <c r="A23" s="12" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" s="12"/>
+      <c r="A24" s="12" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" s="12"/>
+      <c r="A25" s="12" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" s="12"/>
+      <c r="A26" s="12" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" s="12"/>
+      <c r="A27" s="12" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" s="12"/>
+      <c r="A28" s="12" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29" s="12"/>
+      <c r="A29" s="12" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" s="12" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" s="12" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" s="12" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" s="12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" s="12" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" s="12" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" s="12" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" s="12" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" s="12" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" s="12" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" s="12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42" s="12" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A43" s="12" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A44" s="12" t="s">
+        <v>114</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2363,5 +2591,6 @@
     <mergeCell ref="A8:A10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="53" orientation="landscape" horizontalDpi="4294967293" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>